<commit_message>
reinvestment criteria and presentation updates
</commit_message>
<xml_diff>
--- a/dataset/2019-10-15-1001257227.xlsx
+++ b/dataset/2019-10-15-1001257227.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Trsry\Investor Reporting\Term Securitizations\OMFIT 2019-2 Term Securitization\Monthly Servicer Reports\September 2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c9a2edfe12abe1ef/Desktop/NYCDSA/Python Project/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C03E942-EFC5-4EDF-84C0-EAAF5D8185E6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{2C03E942-EFC5-4EDF-84C0-EAAF5D8185E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17C70AE1-503A-4A8C-9274-A50367D6927E}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14856" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (2)" sheetId="3" r:id="rId1"/>
@@ -23,7 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -700,16 +705,16 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -722,39 +727,37 @@
     <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -775,16 +778,16 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
     <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -1110,40 +1113,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H227"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="A232" sqref="A232"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="68" style="2" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="2" max="2" width="21.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.109375" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>168</v>
       </c>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>167</v>
       </c>
@@ -1151,7 +1154,7 @@
         <v>43709</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>166</v>
       </c>
@@ -1159,7 +1162,7 @@
         <v>43738</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>165</v>
       </c>
@@ -1167,7 +1170,7 @@
         <v>43753</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>164</v>
       </c>
@@ -1175,7 +1178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>163</v>
       </c>
@@ -1183,15 +1186,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G10" s="6"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>161</v>
       </c>
@@ -1199,7 +1202,7 @@
         <v>43708</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>160</v>
       </c>
@@ -1207,10 +1210,10 @@
         <v>43728</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" s="7"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B17" s="8" t="s">
         <v>159</v>
       </c>
@@ -1227,7 +1230,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>154</v>
       </c>
@@ -1247,7 +1250,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B19" s="8" t="s">
         <v>147</v>
       </c>
@@ -1261,7 +1264,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>144</v>
       </c>
@@ -1278,7 +1281,7 @@
         <v>49962</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>143</v>
       </c>
@@ -1295,7 +1298,7 @@
         <v>49962</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>142</v>
       </c>
@@ -1312,7 +1315,7 @@
         <v>49962</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>141</v>
       </c>
@@ -1329,7 +1332,7 @@
         <v>49962</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>140</v>
       </c>
@@ -1344,7 +1347,7 @@
       <c r="D24" s="19"/>
       <c r="E24" s="19"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>150</v>
       </c>
@@ -1357,7 +1360,7 @@
       <c r="D25" s="19"/>
       <c r="E25" s="19"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>149</v>
       </c>
@@ -1372,12 +1375,12 @@
       <c r="D26" s="19"/>
       <c r="E26" s="19"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B29" s="21"/>
       <c r="C29" s="21" t="s">
         <v>125</v>
@@ -1390,7 +1393,7 @@
       <c r="G29" s="21"/>
       <c r="H29" s="21"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B30" s="21" t="s">
         <v>147</v>
       </c>
@@ -1409,7 +1412,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>144</v>
       </c>
@@ -1427,11 +1430,11 @@
         <v>1</v>
       </c>
       <c r="G31" s="15"/>
-      <c r="H31" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H31" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>143</v>
       </c>
@@ -1449,11 +1452,11 @@
         <v>1</v>
       </c>
       <c r="G32" s="15"/>
-      <c r="H32" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H32" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>142</v>
       </c>
@@ -1471,33 +1474,33 @@
         <v>1</v>
       </c>
       <c r="G33" s="15"/>
-      <c r="H33" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H33" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>141</v>
       </c>
       <c r="B34" s="16">
         <v>98050000</v>
       </c>
-      <c r="C34" s="24">
+      <c r="C34" s="23">
         <v>1</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="16">
         <v>98050000</v>
       </c>
-      <c r="F34" s="24">
+      <c r="F34" s="23">
         <v>1</v>
       </c>
       <c r="G34" s="15"/>
-      <c r="H34" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H34" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>140</v>
       </c>
@@ -1515,16 +1518,16 @@
       <c r="F35" s="22">
         <v>1</v>
       </c>
-      <c r="H35" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H35" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>138</v>
       </c>
@@ -1532,7 +1535,7 @@
         <v>947374173.75999999</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>137</v>
       </c>
@@ -1540,7 +1543,7 @@
         <v>-21056174</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>39</v>
       </c>
@@ -1548,7 +1551,7 @@
         <v>-57935.79</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>136</v>
       </c>
@@ -1556,7 +1559,7 @@
         <v>-182108.59</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>135</v>
       </c>
@@ -1564,7 +1567,7 @@
         <v>-25479567.760000002</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>134</v>
       </c>
@@ -1572,7 +1575,13 @@
         <v>39717615.670000002</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F46" s="9"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F47" s="9"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>133</v>
       </c>
@@ -1580,7 +1589,7 @@
         <v>7114158.8899999997</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>132</v>
       </c>
@@ -1588,7 +1597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>131</v>
       </c>
@@ -1596,7 +1605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>130</v>
       </c>
@@ -1604,7 +1613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>129</v>
       </c>
@@ -1612,15 +1621,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F53" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F53" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>127</v>
       </c>
@@ -1629,12 +1638,12 @@
         <v>947430162.17999995</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C57" s="8" t="s">
         <v>125</v>
       </c>
@@ -1642,40 +1651,40 @@
         <v>124</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C58" s="27">
+      <c r="C58" s="25">
         <v>26.91</v>
       </c>
-      <c r="F58" s="27">
+      <c r="F58" s="25">
         <v>26.9</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C59" s="28">
+      <c r="C59" s="26">
         <v>629</v>
       </c>
-      <c r="F59" s="28">
+      <c r="F59" s="26">
         <v>629</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C60" s="28">
+      <c r="C60" s="26">
         <v>48</v>
       </c>
-      <c r="F60" s="28">
+      <c r="F60" s="26">
         <v>47</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>121</v>
       </c>
@@ -1688,114 +1697,114 @@
         <v>947430162.17999995</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C62" s="28">
+      <c r="C62" s="26">
         <v>127037</v>
       </c>
-      <c r="D62" s="28"/>
-      <c r="E62" s="28"/>
-      <c r="F62" s="28">
+      <c r="D62" s="26"/>
+      <c r="E62" s="26"/>
+      <c r="F62" s="26">
         <v>126478</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C63" s="28"/>
-      <c r="D63" s="28"/>
-      <c r="E63" s="28"/>
-      <c r="F63" s="28"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C63" s="26"/>
+      <c r="D63" s="26"/>
+      <c r="E63" s="26"/>
+      <c r="F63" s="26"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C64" s="28"/>
-      <c r="D64" s="28"/>
-      <c r="E64" s="28"/>
-      <c r="F64" s="28"/>
+      <c r="C64" s="26"/>
+      <c r="D64" s="26"/>
+      <c r="E64" s="26"/>
+      <c r="F64" s="26"/>
       <c r="H64" s="14"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C65" s="27">
+      <c r="C65" s="25">
         <v>27.16</v>
       </c>
-      <c r="D65" s="28"/>
-      <c r="E65" s="28"/>
-      <c r="F65" s="28"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D65" s="26"/>
+      <c r="E65" s="26"/>
+      <c r="F65" s="26"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C66" s="28">
+      <c r="C66" s="26">
         <v>623</v>
       </c>
-      <c r="D66" s="28"/>
-      <c r="E66" s="28"/>
-      <c r="F66" s="28"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D66" s="26"/>
+      <c r="E66" s="26"/>
+      <c r="F66" s="26"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C67" s="23">
+      <c r="C67" s="9">
         <v>46633904.100000001</v>
       </c>
-      <c r="D67" s="28"/>
-      <c r="E67" s="28"/>
-      <c r="F67" s="28"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D67" s="26"/>
+      <c r="E67" s="26"/>
+      <c r="F67" s="26"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C68" s="28">
+      <c r="C68" s="26">
         <v>4628</v>
       </c>
-      <c r="D68" s="28"/>
-      <c r="E68" s="28"/>
-      <c r="F68" s="28"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C69" s="28"/>
-      <c r="D69" s="28"/>
-      <c r="E69" s="28"/>
-      <c r="F69" s="28"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="29" t="s">
+      <c r="D68" s="26"/>
+      <c r="E68" s="26"/>
+      <c r="F68" s="26"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C69" s="26"/>
+      <c r="D69" s="26"/>
+      <c r="E69" s="26"/>
+      <c r="F69" s="26"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="C70" s="28"/>
-      <c r="D70" s="28"/>
-      <c r="E70" s="28"/>
-      <c r="F70" s="28"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="29" t="s">
+      <c r="C70" s="26"/>
+      <c r="D70" s="26"/>
+      <c r="E70" s="26"/>
+      <c r="F70" s="26"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="C71" s="28"/>
-      <c r="D71" s="28"/>
-      <c r="E71" s="28"/>
-      <c r="F71" s="28"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C71" s="26"/>
+      <c r="D71" s="26"/>
+      <c r="E71" s="26"/>
+      <c r="F71" s="26"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>116</v>
       </c>
@@ -1803,7 +1812,7 @@
         <v>21056174</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>115</v>
       </c>
@@ -1811,7 +1820,7 @@
         <v>182108.59</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>114</v>
       </c>
@@ -1819,15 +1828,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="F79" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F79" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>112</v>
       </c>
@@ -1836,16 +1845,16 @@
         <v>21238282.59</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F81" s="9"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>111</v>
       </c>
       <c r="F82" s="9"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>110</v>
       </c>
@@ -1853,15 +1862,15 @@
         <v>20422691.079999998</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="F84" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F84" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>108</v>
       </c>
@@ -1870,10 +1879,10 @@
         <v>20422691.079999998</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F86" s="9"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>107</v>
       </c>
@@ -1881,7 +1890,7 @@
         <v>-14238047.91</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>106</v>
       </c>
@@ -1889,24 +1898,24 @@
         <v>-7114158.8899999997</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F89" s="26">
+      <c r="F89" s="24">
         <v>-2763174.67</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F90" s="14">
         <f>SUM(F87:F89)</f>
         <v>-24115381.469999999</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F91" s="14"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>104</v>
       </c>
@@ -1914,7 +1923,7 @@
         <v>11706.18</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>103</v>
       </c>
@@ -1922,7 +1931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>102</v>
       </c>
@@ -1930,7 +1939,7 @@
         <v>2536.0300000000002</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>76</v>
       </c>
@@ -1938,10 +1947,10 @@
         <v>4500000</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F97" s="9"/>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>101</v>
       </c>
@@ -1949,10 +1958,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F99" s="9"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>100</v>
       </c>
@@ -1961,20 +1970,20 @@
         <v>22059834.410000004</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="30" t="s">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A104" s="28" t="s">
         <v>98</v>
       </c>
       <c r="F104" s="9">
         <v>833.33</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>97</v>
       </c>
@@ -1982,7 +1991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>96</v>
       </c>
@@ -1990,7 +1999,7 @@
         <v>7236.89</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>95</v>
       </c>
@@ -1998,7 +2007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>94</v>
       </c>
@@ -2006,7 +2015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>93</v>
       </c>
@@ -2014,7 +2023,7 @@
         <v>1363429.87</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>92</v>
       </c>
@@ -2022,7 +2031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>91</v>
       </c>
@@ -2030,7 +2039,7 @@
         <v>207828.13</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>90</v>
       </c>
@@ -2038,7 +2047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>89</v>
       </c>
@@ -2046,7 +2055,7 @@
         <v>144472.4</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>88</v>
       </c>
@@ -2054,7 +2063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>87</v>
       </c>
@@ -2062,7 +2071,7 @@
         <v>264735</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>86</v>
       </c>
@@ -2070,7 +2079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>85</v>
       </c>
@@ -2079,7 +2088,7 @@
       </c>
       <c r="H117" s="9"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>84</v>
       </c>
@@ -2088,7 +2097,7 @@
       </c>
       <c r="H118" s="9"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>83</v>
       </c>
@@ -2097,7 +2106,7 @@
       </c>
       <c r="H119" s="14"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>82</v>
       </c>
@@ -2105,7 +2114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>81</v>
       </c>
@@ -2113,16 +2122,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F122" s="26">
+      <c r="F122" s="24">
         <v>15571298.789999999</v>
       </c>
       <c r="H122" s="14"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>79</v>
       </c>
@@ -2131,12 +2140,12 @@
         <v>22059834.41</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>77</v>
       </c>
@@ -2144,7 +2153,7 @@
         <v>4500000</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>76</v>
       </c>
@@ -2152,7 +2161,7 @@
         <v>-4500000</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>75</v>
       </c>
@@ -2160,7 +2169,7 @@
         <v>4500000</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>74</v>
       </c>
@@ -2168,7 +2177,7 @@
         <v>4500000</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>73</v>
       </c>
@@ -2176,7 +2185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>72</v>
       </c>
@@ -2184,12 +2193,12 @@
         <v>4500000</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>70</v>
       </c>
@@ -2197,7 +2206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>69</v>
       </c>
@@ -2205,7 +2214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>68</v>
       </c>
@@ -2213,10 +2222,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F138" s="9"/>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>67</v>
       </c>
@@ -2224,13 +2233,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F140" s="9"/>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>65</v>
       </c>
@@ -2238,7 +2247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>64</v>
       </c>
@@ -2246,7 +2255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>63</v>
       </c>
@@ -2254,7 +2263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>62</v>
       </c>
@@ -2262,7 +2271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>61</v>
       </c>
@@ -2270,7 +2279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>60</v>
       </c>
@@ -2278,7 +2287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>59</v>
       </c>
@@ -2286,16 +2295,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F148" s="9"/>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149" s="3" t="s">
         <v>58</v>
       </c>
       <c r="F149" s="9"/>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
         <v>57</v>
       </c>
@@ -2303,7 +2312,7 @@
         <v>947430162.17999995</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>56</v>
       </c>
@@ -2311,15 +2320,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F153" s="26">
+      <c r="F153" s="24">
         <v>900000000</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>54</v>
       </c>
@@ -2327,7 +2336,7 @@
         <v>47430162.18</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>53</v>
       </c>
@@ -2335,7 +2344,7 @@
         <v>47374173.759999998</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>26</v>
       </c>
@@ -2343,289 +2352,289 @@
         <v>5</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A158" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C159" s="31" t="s">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C159" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="D159" s="31" t="s">
+      <c r="D159" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="E159" s="31" t="s">
+      <c r="E159" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="F159" s="31" t="s">
+      <c r="F159" s="29" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C160" s="28">
+      <c r="C160" s="26">
         <v>122501</v>
       </c>
-      <c r="D160" s="32">
+      <c r="D160" s="30">
         <v>0.96860000000000002</v>
       </c>
-      <c r="E160" s="23">
+      <c r="E160" s="9">
         <v>917463683.63</v>
       </c>
-      <c r="F160" s="32">
+      <c r="F160" s="30">
         <v>0.96840000000000004</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C161" s="28">
+      <c r="C161" s="26">
         <v>3963</v>
       </c>
-      <c r="D161" s="32">
+      <c r="D161" s="30">
         <v>3.1300000000000001E-2</v>
       </c>
-      <c r="E161" s="23">
+      <c r="E161" s="9">
         <v>29859204.25</v>
       </c>
-      <c r="F161" s="32">
+      <c r="F161" s="30">
         <v>3.15E-2</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C162" s="28">
+      <c r="C162" s="26">
         <v>13</v>
       </c>
-      <c r="D162" s="32">
+      <c r="D162" s="30">
         <v>1E-4</v>
       </c>
-      <c r="E162" s="23">
+      <c r="E162" s="9">
         <v>93857.94</v>
       </c>
-      <c r="F162" s="32">
+      <c r="F162" s="30">
         <v>1E-4</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C163" s="28">
+      <c r="C163" s="26">
         <v>1</v>
       </c>
-      <c r="D163" s="32">
-        <v>0</v>
-      </c>
-      <c r="E163" s="23">
+      <c r="D163" s="30">
+        <v>0</v>
+      </c>
+      <c r="E163" s="9">
         <v>13416.36</v>
       </c>
-      <c r="F163" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F163" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C164" s="28">
-        <v>0</v>
-      </c>
-      <c r="D164" s="32">
-        <v>0</v>
-      </c>
-      <c r="E164" s="23">
-        <v>0</v>
-      </c>
-      <c r="F164" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C164" s="26">
+        <v>0</v>
+      </c>
+      <c r="D164" s="30">
+        <v>0</v>
+      </c>
+      <c r="E164" s="9">
+        <v>0</v>
+      </c>
+      <c r="F164" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C165" s="33">
-        <v>0</v>
-      </c>
-      <c r="D165" s="34">
-        <v>0</v>
-      </c>
-      <c r="E165" s="25">
-        <v>0</v>
-      </c>
-      <c r="F165" s="34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C166" s="28">
+      <c r="C165" s="31">
+        <v>0</v>
+      </c>
+      <c r="D165" s="32">
+        <v>0</v>
+      </c>
+      <c r="E165" s="24">
+        <v>0</v>
+      </c>
+      <c r="F165" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C166" s="26">
         <f>SUM(C160:C165)</f>
         <v>126478</v>
       </c>
-      <c r="D166" s="35">
+      <c r="D166" s="33">
         <f>SUM(D160:D165)</f>
         <v>1</v>
       </c>
-      <c r="E166" s="23">
+      <c r="E166" s="9">
         <f>SUM(E160:E165)</f>
         <v>947430162.18000007</v>
       </c>
-      <c r="F166" s="35">
+      <c r="F166" s="33">
         <f>SUM(F160:F165)</f>
         <v>1</v>
       </c>
-      <c r="G166" s="28"/>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C167" s="28"/>
-      <c r="D167" s="32"/>
+      <c r="G166" s="26"/>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C167" s="26"/>
+      <c r="D167" s="30"/>
       <c r="E167" s="9"/>
-      <c r="F167" s="32"/>
-    </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F167" s="30"/>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A168" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C168" s="28"/>
-      <c r="D168" s="32"/>
+      <c r="C168" s="26"/>
+      <c r="D168" s="30"/>
       <c r="E168" s="9"/>
       <c r="F168" s="9"/>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C169" s="28"/>
-      <c r="D169" s="32"/>
+      <c r="C169" s="26"/>
+      <c r="D169" s="30"/>
       <c r="E169" s="9"/>
       <c r="F169" s="9">
         <v>947374173.75999999</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C170" s="28"/>
-      <c r="D170" s="32"/>
+      <c r="C170" s="26"/>
+      <c r="D170" s="30"/>
       <c r="E170" s="9"/>
       <c r="F170" s="9">
         <v>57935.79</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C171" s="28"/>
-      <c r="D171" s="32"/>
+      <c r="C171" s="26"/>
+      <c r="D171" s="30"/>
       <c r="E171" s="9"/>
-      <c r="F171" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F171" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C172" s="28"/>
-      <c r="D172" s="32"/>
+      <c r="C172" s="26"/>
+      <c r="D172" s="30"/>
       <c r="E172" s="9"/>
-      <c r="F172" s="36">
+      <c r="F172" s="34">
         <v>57935.79</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C173" s="28"/>
-      <c r="D173" s="32"/>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C173" s="26"/>
+      <c r="D173" s="30"/>
       <c r="E173" s="9"/>
       <c r="F173" s="9"/>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C174" s="28"/>
-      <c r="D174" s="32"/>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C174" s="26"/>
+      <c r="D174" s="30"/>
       <c r="E174" s="9"/>
-      <c r="F174" s="32"/>
-    </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F174" s="30"/>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C175" s="28"/>
-      <c r="D175" s="32"/>
+      <c r="C175" s="26"/>
+      <c r="D175" s="30"/>
       <c r="E175" s="9"/>
-      <c r="F175" s="37">
+      <c r="F175" s="35">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C176" s="28"/>
-      <c r="D176" s="32"/>
+      <c r="C176" s="26"/>
+      <c r="D176" s="30"/>
       <c r="E176" s="9"/>
-      <c r="F176" s="37" t="s">
+      <c r="F176" s="35" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C177" s="28"/>
-      <c r="D177" s="32"/>
+      <c r="C177" s="26"/>
+      <c r="D177" s="30"/>
       <c r="E177" s="9"/>
-      <c r="F177" s="37" t="s">
+      <c r="F177" s="35" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C178" s="28"/>
-      <c r="D178" s="32"/>
+      <c r="C178" s="26"/>
+      <c r="D178" s="30"/>
       <c r="E178" s="9"/>
-      <c r="F178" s="38">
+      <c r="F178" s="36">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A179" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C179" s="28"/>
-      <c r="D179" s="32"/>
+      <c r="C179" s="26"/>
+      <c r="D179" s="30"/>
       <c r="E179" s="9"/>
-      <c r="F179" s="37" t="s">
+      <c r="F179" s="35" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A180" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C180" s="28"/>
-      <c r="D180" s="32"/>
+      <c r="C180" s="26"/>
+      <c r="D180" s="30"/>
       <c r="E180" s="9"/>
-      <c r="F180" s="37" t="s">
+      <c r="F180" s="35" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A182" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C183" s="8" t="s">
         <v>29</v>
       </c>
@@ -2639,7 +2648,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
         <v>174</v>
       </c>
@@ -2652,17 +2661,17 @@
       <c r="E184" s="12">
         <v>67.5</v>
       </c>
-      <c r="F184" s="39" t="s">
+      <c r="F184" s="37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C185" s="40"/>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C185" s="38"/>
       <c r="D185" s="15"/>
       <c r="E185" s="15"/>
       <c r="F185" s="8"/>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
         <v>25</v>
       </c>
@@ -2675,11 +2684,11 @@
       <c r="E186" s="12">
         <v>0.5</v>
       </c>
-      <c r="F186" s="39" t="s">
+      <c r="F186" s="37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
         <v>24</v>
       </c>
@@ -2692,11 +2701,11 @@
       <c r="E187" s="12">
         <v>6</v>
       </c>
-      <c r="F187" s="39" t="s">
+      <c r="F187" s="37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A188" s="2" t="s">
         <v>23</v>
       </c>
@@ -2709,11 +2718,11 @@
       <c r="E188" s="12">
         <v>20</v>
       </c>
-      <c r="F188" s="39" t="s">
+      <c r="F188" s="37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A189" s="2" t="s">
         <v>22</v>
       </c>
@@ -2726,11 +2735,11 @@
       <c r="E189" s="12">
         <v>45</v>
       </c>
-      <c r="F189" s="39" t="s">
+      <c r="F189" s="37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A190" s="2" t="s">
         <v>21</v>
       </c>
@@ -2743,11 +2752,11 @@
       <c r="E190" s="12">
         <v>70</v>
       </c>
-      <c r="F190" s="39" t="s">
+      <c r="F190" s="37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A191" s="2" t="s">
         <v>20</v>
       </c>
@@ -2760,11 +2769,11 @@
       <c r="E191" s="12">
         <v>90</v>
       </c>
-      <c r="F191" s="39" t="s">
+      <c r="F191" s="37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A192" s="2" t="s">
         <v>19</v>
       </c>
@@ -2777,17 +2786,17 @@
       <c r="E192" s="15">
         <v>1</v>
       </c>
-      <c r="F192" s="39" t="s">
+      <c r="F192" s="37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C193" s="15"/>
       <c r="D193" s="15"/>
       <c r="E193" s="15"/>
-      <c r="F193" s="39"/>
-    </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F193" s="37"/>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
         <v>18</v>
       </c>
@@ -2800,11 +2809,11 @@
       <c r="E194" s="12">
         <v>40</v>
       </c>
-      <c r="F194" s="39" t="s">
+      <c r="F194" s="37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A195" s="2" t="s">
         <v>17</v>
       </c>
@@ -2817,11 +2826,11 @@
       <c r="E195" s="12">
         <v>15</v>
       </c>
-      <c r="F195" s="39" t="s">
+      <c r="F195" s="37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A196" s="2" t="s">
         <v>16</v>
       </c>
@@ -2834,17 +2843,17 @@
       <c r="E196" s="12">
         <v>12.5</v>
       </c>
-      <c r="F196" s="39" t="s">
+      <c r="F196" s="37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C197" s="15"/>
       <c r="D197" s="15"/>
       <c r="E197" s="15"/>
-      <c r="F197" s="39"/>
-    </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F197" s="37"/>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A198" s="2" t="s">
         <v>15</v>
       </c>
@@ -2857,28 +2866,28 @@
       <c r="E198" s="12">
         <v>23.5</v>
       </c>
-      <c r="F198" s="39" t="s">
+      <c r="F198" s="37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A199" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C199" s="13">
         <v>48</v>
       </c>
-      <c r="D199" s="41">
+      <c r="D199" s="39">
         <v>47</v>
       </c>
-      <c r="E199" s="41">
+      <c r="E199" s="39">
         <v>58</v>
       </c>
-      <c r="F199" s="39" t="s">
+      <c r="F199" s="37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A200" s="2" t="s">
         <v>13</v>
       </c>
@@ -2891,15 +2900,15 @@
       <c r="E200" s="12">
         <v>7.5</v>
       </c>
-      <c r="F200" s="39" t="s">
+      <c r="F200" s="37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A201" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C201" s="42">
+      <c r="C201" s="40">
         <v>0.92</v>
       </c>
       <c r="D201" s="12">
@@ -2908,126 +2917,126 @@
       <c r="E201" s="12">
         <v>4</v>
       </c>
-      <c r="F201" s="39" t="s">
+      <c r="F201" s="37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C202" s="43"/>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C202" s="41"/>
       <c r="D202" s="15"/>
       <c r="E202" s="15"/>
-      <c r="F202" s="39"/>
-    </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F202" s="37"/>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A203" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C203" s="43"/>
+      <c r="C203" s="41"/>
       <c r="D203" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E203" s="15"/>
-      <c r="F203" s="39"/>
-    </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F203" s="37"/>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A204" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C204" s="43"/>
+      <c r="C204" s="41"/>
       <c r="D204" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E204" s="15"/>
-      <c r="F204" s="39"/>
-    </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F204" s="37"/>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A205" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C205" s="43"/>
+      <c r="C205" s="41"/>
       <c r="D205" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E205" s="19"/>
       <c r="F205" s="19"/>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A206" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C206" s="43"/>
+      <c r="C206" s="41"/>
       <c r="D206" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E206" s="19"/>
       <c r="F206" s="19"/>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A207" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C207" s="14">
         <v>0</v>
       </c>
-      <c r="D207" s="44">
+      <c r="D207" s="42">
         <v>0</v>
       </c>
       <c r="E207" s="14">
         <v>189474834.75</v>
       </c>
-      <c r="F207" s="39" t="s">
+      <c r="F207" s="37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A208" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C208" s="45"/>
+      <c r="C208" s="43"/>
       <c r="D208" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="E208" s="27">
+      <c r="E208" s="25">
         <v>95</v>
       </c>
-      <c r="F208" s="39" t="s">
+      <c r="F208" s="37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C209" s="45"/>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C209" s="43"/>
       <c r="D209" s="19"/>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A210" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C212" s="32"/>
-      <c r="E212" s="32"/>
+      <c r="C212" s="30"/>
+      <c r="E212" s="30"/>
       <c r="F212" s="19" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A213" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D213" s="27">
+      <c r="D213" s="25">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E213" s="27">
+      <c r="E213" s="25">
         <v>17</v>
       </c>
       <c r="F213" s="19" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A214" s="2" t="s">
         <v>1</v>
       </c>
@@ -3035,12 +3044,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A216" s="3" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C217" s="8" t="s">
         <v>180</v>
       </c>
@@ -3054,115 +3063,115 @@
         <v>183</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A218" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C218" s="32">
+      <c r="C218" s="30">
         <v>3.1399999999999997E-2</v>
       </c>
-      <c r="D218" s="46">
+      <c r="D218" s="44">
         <v>0.99957379999999996</v>
       </c>
-      <c r="E218" s="48">
+      <c r="E218" s="46">
         <v>651042407</v>
       </c>
-      <c r="F218" s="32">
+      <c r="F218" s="30">
         <v>0.44800000000000001</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A219" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="C219" s="32">
+      <c r="C219" s="30">
         <v>3.4099999999999998E-2</v>
       </c>
-      <c r="D219" s="46">
+      <c r="D219" s="44">
         <v>0.99965800000000005</v>
       </c>
-      <c r="E219" s="48">
+      <c r="E219" s="46">
         <v>91388734</v>
       </c>
-      <c r="F219" s="32">
+      <c r="F219" s="30">
         <v>6.2899999999999998E-2</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A220" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C220" s="32">
+      <c r="C220" s="30">
         <v>3.6600000000000001E-2</v>
       </c>
-      <c r="D220" s="46">
+      <c r="D220" s="44">
         <v>0.99978350000000005</v>
       </c>
-      <c r="E220" s="48">
+      <c r="E220" s="46">
         <v>59197181</v>
       </c>
-      <c r="F220" s="32">
+      <c r="F220" s="30">
         <v>4.07E-2</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A221" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C221" s="32">
+      <c r="C221" s="30">
         <v>4.0500000000000001E-2</v>
       </c>
-      <c r="D221" s="46">
+      <c r="D221" s="44">
         <v>0.99952280000000004</v>
       </c>
-      <c r="E221" s="48">
+      <c r="E221" s="46">
         <v>98003211</v>
       </c>
-      <c r="F221" s="32">
+      <c r="F221" s="30">
         <v>6.7400000000000002E-2</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A222" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C222" s="34"/>
-      <c r="D222" s="49"/>
-      <c r="E222" s="50">
+      <c r="C222" s="32"/>
+      <c r="D222" s="47"/>
+      <c r="E222" s="48">
         <v>553603277</v>
       </c>
-      <c r="F222" s="34">
+      <c r="F222" s="32">
         <v>0.38090000000000002</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C223" s="45"/>
-      <c r="D223" s="46"/>
-      <c r="E223" s="48">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C223" s="43"/>
+      <c r="D223" s="44"/>
+      <c r="E223" s="46">
         <f>SUM(E218:E222)</f>
         <v>1453234810</v>
       </c>
-      <c r="F223" s="51">
+      <c r="F223" s="49">
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C224" s="45"/>
-      <c r="D224" s="46"/>
-      <c r="E224" s="47"/>
-      <c r="F224" s="35"/>
-    </row>
-    <row r="225" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C225" s="45"/>
-      <c r="D225" s="46"/>
-      <c r="E225" s="47"/>
-    </row>
-    <row r="226" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D226" s="35"/>
-      <c r="E226" s="47"/>
-    </row>
-    <row r="227" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E227" s="47"/>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C224" s="43"/>
+      <c r="D224" s="44"/>
+      <c r="E224" s="45"/>
+      <c r="F224" s="33"/>
+    </row>
+    <row r="225" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C225" s="43"/>
+      <c r="D225" s="44"/>
+      <c r="E225" s="45"/>
+    </row>
+    <row r="226" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="D226" s="33"/>
+      <c r="E226" s="45"/>
+    </row>
+    <row r="227" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E227" s="45"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>